<commit_message>
Minor post-processing procedure updates
</commit_message>
<xml_diff>
--- a/projects/puerto_rico_stoch/data/data_A.xlsx
+++ b/projects/puerto_rico_stoch/data/data_A.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B3A90A-27C7-4F40-BE66-592109CFC6C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBCF1A1-1434-4345-B423-D6E7928E08F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="941" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="941" firstSheet="3" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="4" r:id="rId1"/>
@@ -13,9 +13,9 @@
     <sheet name="timesOfDay" sheetId="18" r:id="rId3"/>
     <sheet name="Connections" sheetId="1" r:id="rId4"/>
     <sheet name="ConnectionsExisting" sheetId="2" r:id="rId5"/>
-    <sheet name="Fuels" sheetId="6" r:id="rId6"/>
-    <sheet name="Demand" sheetId="3" r:id="rId7"/>
-    <sheet name="DiscountRate" sheetId="5" r:id="rId8"/>
+    <sheet name="Demand" sheetId="3" r:id="rId6"/>
+    <sheet name="DiscountRate" sheetId="5" r:id="rId7"/>
+    <sheet name="Fuels" sheetId="6" r:id="rId8"/>
     <sheet name="PowerPlants" sheetId="8" r:id="rId9"/>
     <sheet name="FuelsExisting" sheetId="7" r:id="rId10"/>
     <sheet name="PowerPlantsPerformance" sheetId="12" r:id="rId11"/>
@@ -3599,7 +3599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:I1048576"/>
     </sheetView>
   </sheetViews>
@@ -5287,7 +5287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6192,6 +6192,180 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2016</v>
+      </c>
+      <c r="B3" s="30">
+        <v>75.239999999999995</v>
+      </c>
+      <c r="C3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2021</v>
+      </c>
+      <c r="B4" s="30">
+        <v>66.489999999999995</v>
+      </c>
+      <c r="C4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2026</v>
+      </c>
+      <c r="B5" s="30">
+        <v>67.28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2031</v>
+      </c>
+      <c r="B6" s="30">
+        <v>65.319999999999993</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2036</v>
+      </c>
+      <c r="B7" s="30">
+        <v>63.75</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2041</v>
+      </c>
+      <c r="B8" s="30">
+        <v>63.75</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="29">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0.09</v>
+      </c>
+      <c r="B3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
@@ -6501,180 +6675,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2016</v>
-      </c>
-      <c r="B3" s="30">
-        <v>75.239999999999995</v>
-      </c>
-      <c r="C3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2021</v>
-      </c>
-      <c r="B4" s="30">
-        <v>66.489999999999995</v>
-      </c>
-      <c r="C4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>2026</v>
-      </c>
-      <c r="B5" s="30">
-        <v>67.28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2031</v>
-      </c>
-      <c r="B6" s="30">
-        <v>65.319999999999993</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>2036</v>
-      </c>
-      <c r="B7" s="30">
-        <v>63.75</v>
-      </c>
-      <c r="C7" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>2041</v>
-      </c>
-      <c r="B8" s="30">
-        <v>63.75</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" s="29">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>0.09</v>
-      </c>
-      <c r="B3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>